<commit_message>
HDM - Culminacion de flujo de servicio
</commit_message>
<xml_diff>
--- a/informes_generados/Olmos_Muestra_3231808.xlsx
+++ b/informes_generados/Olmos_Muestra_3231808.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>arandano</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -608,7 +608,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Alimentos</t>
+          <t>arandano</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>